<commit_message>
updated excel file and ran python script
</commit_message>
<xml_diff>
--- a/create_json/musicsketch_faqs.xlsx
+++ b/create_json/musicsketch_faqs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnwalecka/jwalecka.github.io/create_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{88D23569-81E8-6048-AFE4-81FC8890AC3B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BCDA9C-67F0-054F-9B4F-7289EC2545FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3900" yWindow="2200" windowWidth="29280" windowHeight="18900" xr2:uid="{E9479D6A-3051-CF47-9481-B1BE55C8F822}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="105" uniqueCount="77">
   <si>
     <t>Overview</t>
   </si>
@@ -130,9 +130,6 @@
   </si>
   <si>
     <t xml:space="preserve">Only songs in the My Songs folder can be edited. To edit Demo Songs and Accompaniments you have to duplicate them first, which will add them to the My Songs folder. </t>
-  </si>
-  <si>
-    <t>Is there a way to undo my last change?</t>
   </si>
   <si>
     <t>To undo an action or sequence of actions, shake your iPhone and select Undo.</t>
@@ -327,6 +324,12 @@
       </rPr>
       <t>ard (DIBO) allows for quick and easy note entry, and the additional UI adapts additional notation elements.  To achieve these goals we oriented on a design point around notation critical for Lead Sheets.  While our platform doesn’t capture the entire functionality of desktop music publishing software, we think the tradeoff for speed, simplicity, and accessibility is more than worth it. /nWe appreciate and welcome input from all of our users.  New capabilities are in the works, but we will continue to make trade-offs to ensure that the MusicSketch App remains uncluttered and easy to use, allowing musicians at all levels to focus on their creative ideas.</t>
     </r>
+  </si>
+  <si>
+    <t>Is there a way to undo my last song change?</t>
+  </si>
+  <si>
+    <t>Is there a way to undo my last notation change?</t>
   </si>
 </sst>
 </file>
@@ -698,12 +701,13 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="22.5" customWidth="1"/>
+    <col min="1" max="1" width="22.5" customWidth="1"/>
+    <col min="2" max="2" width="45.5" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
   </cols>
   <sheetData>
@@ -715,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -803,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -888,208 +892,208 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>33</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B18" s="1" t="s">
         <v>34</v>
       </c>
-      <c r="B18" s="1" t="s">
+      <c r="C18" s="1" t="s">
         <v>35</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B19" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="C19" s="1" t="s">
         <v>37</v>
-      </c>
-      <c r="C19" s="1" t="s">
-        <v>38</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B20" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="C20" s="1" t="s">
         <v>39</v>
-      </c>
-      <c r="C20" s="1" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B21" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>41</v>
-      </c>
-      <c r="C21" s="1" t="s">
-        <v>42</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B22" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="C22" s="1" t="s">
         <v>43</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B23" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C23" s="1" t="s">
         <v>45</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A24" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B24" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="C24" s="1" t="s">
         <v>47</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>48</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B25" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C25" s="1" t="s">
         <v>49</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>50</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B26" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="C26" s="1" t="s">
         <v>51</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
-        <v>32</v>
+        <v>76</v>
       </c>
       <c r="C27" s="1" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>54</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>55</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>57</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>58</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>59</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>61</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>62</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>63</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>64</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>65</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>65</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>66</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>67</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>70</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>72</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
ran python script again
</commit_message>
<xml_diff>
--- a/create_json/musicsketch_faqs.xlsx
+++ b/create_json/musicsketch_faqs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnwalecka/jwalecka.github.io/create_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{40BCDA9C-67F0-054F-9B4F-7289EC2545FC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0767E68-C5D9-7B46-A258-15A0E2BD4507}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3900" yWindow="2200" windowWidth="29280" windowHeight="18900" xr2:uid="{E9479D6A-3051-CF47-9481-B1BE55C8F822}"/>
+    <workbookView xWindow="3900" yWindow="2200" windowWidth="31520" windowHeight="18900" xr2:uid="{E9479D6A-3051-CF47-9481-B1BE55C8F822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -190,9 +190,6 @@
   </si>
   <si>
     <t>Add notes above or below the staff by tapping the small DIBO icons at the top and bottom of the DIBO, or by swiping up or down on the DIBO.</t>
-  </si>
-  <si>
-    <t>To undo an action or sequence of actions, shake the iPhone and select undo from the pop up menu.  Most, but not all actions can be undone.</t>
   </si>
   <si>
     <t>What limits to notation are there in the app?</t>
@@ -330,6 +327,9 @@
   </si>
   <si>
     <t>Is there a way to undo my last notation change?</t>
+  </si>
+  <si>
+    <t>To undo an action or sequence of actions, shake the iPhone and select undo from the pop up menu.  Most, but not all notation related actions can be undone.</t>
   </si>
 </sst>
 </file>
@@ -701,7 +701,7 @@
   <dimension ref="A1:C35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B31" sqref="B31"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -719,7 +719,7 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -807,7 +807,7 @@
         <v>16</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -892,7 +892,7 @@
         <v>19</v>
       </c>
       <c r="B17" s="1" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C17" s="1" t="s">
         <v>32</v>
@@ -1002,10 +1002,10 @@
         <v>33</v>
       </c>
       <c r="B27" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="C27" s="1" t="s">
         <v>76</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>52</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.2">
@@ -1013,87 +1013,87 @@
         <v>33</v>
       </c>
       <c r="B28" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="C28" s="1" t="s">
         <v>53</v>
-      </c>
-      <c r="C28" s="1" t="s">
-        <v>54</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B29" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="B29" s="1" t="s">
+      <c r="C29" s="1" t="s">
         <v>56</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>57</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A30" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B30" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C30" s="1" t="s">
         <v>58</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A31" s="2" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B31" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C31" s="1" t="s">
         <v>60</v>
-      </c>
-      <c r="C31" s="1" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A32" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="B32" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="B32" s="1" t="s">
+      <c r="C32" s="1" t="s">
         <v>63</v>
-      </c>
-      <c r="C32" s="1" t="s">
-        <v>64</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A33" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="B33" s="1" t="s">
         <v>65</v>
       </c>
-      <c r="B33" s="1" t="s">
+      <c r="C33" s="1" t="s">
         <v>66</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>67</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B34" s="1" t="s">
         <v>68</v>
       </c>
-      <c r="B34" s="1" t="s">
+      <c r="C34" s="1" t="s">
         <v>69</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B35" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="C35" s="1" t="s">
         <v>71</v>
-      </c>
-      <c r="C35" s="1" t="s">
-        <v>72</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
removed duplicate from json file
</commit_message>
<xml_diff>
--- a/create_json/musicsketch_faqs.xlsx
+++ b/create_json/musicsketch_faqs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/johnwalecka/jwalecka.github.io/create_json/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EDD7BE2-2F10-6646-96B6-568C541B98BC}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4CBE5A3-C5B7-614B-81F1-33B97F9BD50D}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="940" yWindow="1800" windowWidth="31520" windowHeight="18900" xr2:uid="{E9479D6A-3051-CF47-9481-B1BE55C8F822}"/>
+    <workbookView xWindow="940" yWindow="1800" windowWidth="33160" windowHeight="20600" xr2:uid="{E9479D6A-3051-CF47-9481-B1BE55C8F822}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="85">
   <si>
     <t>Overview</t>
   </si>
@@ -285,7 +285,10 @@
     <t>You can create and export M4A Audio files or MIDI files by swiping a song title to the right from the song list or selecting the share button in the multi-measure view. Keep in mind the audio conversion process may take longer than you expect!</t>
   </si>
   <si>
-    <t>Placeholder</t>
+    <t>Placeholder 1</t>
+  </si>
+  <si>
+    <t>Placeholder 2</t>
   </si>
 </sst>
 </file>
@@ -648,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AEE1C598-4A4A-AF45-8787-7E798E6670C1}">
   <dimension ref="A1:C39"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="C41" sqref="C41"/>
+    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="125" workbookViewId="0">
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1085,7 +1088,7 @@
         <v>42</v>
       </c>
       <c r="C39" s="1" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>

</xml_diff>